<commit_message>
save latest working version of the code
</commit_message>
<xml_diff>
--- a/eenav_clean.xlsx
+++ b/eenav_clean.xlsx
@@ -436,29 +436,29 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>FIRST NAME</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>LAST NAME</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EE Nav Premium</t>
+          <t>PREMIUM TOTAL</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>SARAH</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Abedi</t>
+          <t>ABEDI</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -468,12 +468,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Lindsey</t>
+          <t>LINDSEY</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ackerman</t>
+          <t>ACKERMAN</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -483,12 +483,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Steven</t>
+          <t>STEVEN</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Agoglia</t>
+          <t>AGOGLIA</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -498,12 +498,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kaylan</t>
+          <t>KAYLAN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Arroyo</t>
+          <t>ARROYO</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -513,12 +513,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Brooke</t>
+          <t>BROOKE</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Arthur</t>
+          <t>ARTHUR</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -528,12 +528,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>JAMIE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Arthur</t>
+          <t>ARTHUR</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -543,12 +543,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Jonathan</t>
+          <t>JONATHAN</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Artigue</t>
+          <t>ARTIGUE</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -558,12 +558,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Cassandra</t>
+          <t>CASSANDRA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ayala Lopez</t>
+          <t>AYALA LOPEZ</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -588,12 +588,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gabriela</t>
+          <t>GABRIELA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Becerra</t>
+          <t>BECERRA</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -603,12 +603,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>RYAN</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Beckley</t>
+          <t>BECKLEY</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -618,12 +618,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Kelly</t>
+          <t>KELLY</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Benini</t>
+          <t>BENINI</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -633,12 +633,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kelsey</t>
+          <t>KELSEY</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bettis Trujillo</t>
+          <t>BETTIS TRUJILLO</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -648,12 +648,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>SAMUEL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Biggers</t>
+          <t>BIGGERS</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -663,12 +663,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>DAVID</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bisignano</t>
+          <t>BISIGNANO</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -678,12 +678,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>RYAN</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bland</t>
+          <t>BLAND</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -693,12 +693,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>ALEX</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Boghossian</t>
+          <t>BOGHOSSIAN</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -708,12 +708,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Terrance</t>
+          <t>TERRANCE</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bovell</t>
+          <t>BOVELL</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -723,12 +723,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Brenda</t>
+          <t>BRENDA</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Cabrera</t>
+          <t>CABRERA</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -738,12 +738,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>MELISSA</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Camberos</t>
+          <t>CAMBEROS</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -753,12 +753,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>JENNIFER</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Carbajal</t>
+          <t>CARBAJAL</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -783,12 +783,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Marissa</t>
+          <t>MARISSA</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Chantorn</t>
+          <t>CHANTORN</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -798,12 +798,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Myra</t>
+          <t>MYRA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Chavez</t>
+          <t>CHAVEZ</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -813,12 +813,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>DAVID</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Chocco</t>
+          <t>CHOCCO</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -828,12 +828,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Yoo Sun Jennifer</t>
+          <t>YOO SUN JENNIFER</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Choi</t>
+          <t>CHOI</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -843,12 +843,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Laura</t>
+          <t>LAURA</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Cholico</t>
+          <t>CHOLICO</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -858,12 +858,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Allison</t>
+          <t>ALLISON</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ciongoli</t>
+          <t>CIONGOLI</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -873,12 +873,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Masha</t>
+          <t>MASHA</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cohen</t>
+          <t>COHEN</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -888,12 +888,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Jenalee</t>
+          <t>JENALEE</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Collins</t>
+          <t>COLLINS</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -903,12 +903,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Pamela</t>
+          <t>PAMELA</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Corey</t>
+          <t>COREY</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -918,12 +918,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Angelica</t>
+          <t>ANGELICA</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Cortez</t>
+          <t>CORTEZ</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -933,12 +933,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Emily</t>
+          <t>EMILY</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Cruz</t>
+          <t>CRUZ</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -948,12 +948,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Caitlyn</t>
+          <t>CAITLYN</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>DAVIS</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -963,12 +963,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Frankie</t>
+          <t>FRANKIE</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>DAVIS</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -993,12 +993,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Desirae</t>
+          <t>DESIRAE</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Desrosiers</t>
+          <t>DESROSIERS</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1008,12 +1008,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Dana</t>
+          <t>DANA</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Donahoe</t>
+          <t>DONAHOE</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1023,12 +1023,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Makayla</t>
+          <t>MAKAYLA</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Edmonds</t>
+          <t>EDMONDS</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1038,12 +1038,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Peter</t>
+          <t>PETER</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ehrenfried</t>
+          <t>EHRENFRIED</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1053,12 +1053,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Izunna</t>
+          <t>IZUNNA</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Ewudo</t>
+          <t>EWUDO</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1068,12 +1068,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Mava</t>
+          <t>MAVA</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Fakoori</t>
+          <t>FAKOORI</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1083,12 +1083,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Samaneh</t>
+          <t>SAMANEH</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Fanaeian</t>
+          <t>FANAEIAN</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1098,12 +1098,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Joanna</t>
+          <t>JOANNA</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Farah</t>
+          <t>FARAH</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1113,12 +1113,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Hayley</t>
+          <t>HAYLEY</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Feuer</t>
+          <t>FEUER</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1128,12 +1128,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Carmen</t>
+          <t>CARMEN</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Flores</t>
+          <t>FLORES</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1143,12 +1143,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Derek</t>
+          <t>DEREK</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Free</t>
+          <t>FREE</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1158,12 +1158,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Carolina</t>
+          <t>CAROLINA</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Gallegos</t>
+          <t>GALLEGOS</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1173,12 +1173,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Antoinette</t>
+          <t>ANTOINETTE</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>GARCIA</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1188,12 +1188,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Toshton</t>
+          <t>TOSHTON</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Garcia</t>
+          <t>GARCIA</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1203,12 +1203,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Jacob</t>
+          <t>JACOB</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Gertler</t>
+          <t>GERTLER</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1218,12 +1218,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Sara</t>
+          <t>SARA</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Ghassemy</t>
+          <t>GHASSEMY</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1233,12 +1233,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Alexa</t>
+          <t>ALEXA</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Gonzalez</t>
+          <t>GONZALEZ</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1248,12 +1248,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Zulema</t>
+          <t>ZULEMA</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Gonzalez Mendez</t>
+          <t>GONZALEZ MENDEZ</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1263,12 +1263,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Dezire</t>
+          <t>DEZIRE</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Gregory-Highshaw</t>
+          <t>GREGORY-HIGHSHAW</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1278,7 +1278,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Alexa</t>
+          <t>ALEXA</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1293,12 +1293,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Daniah</t>
+          <t>DANIAH</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Hamouda</t>
+          <t>HAMOUDA</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1308,12 +1308,12 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Molly</t>
+          <t>MOLLY</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Hanna</t>
+          <t>HANNA</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1323,12 +1323,12 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Katherine</t>
+          <t>KATHERINE</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Hartnett</t>
+          <t>HARTNETT</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1338,12 +1338,12 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>RYAN</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Hatanaka</t>
+          <t>HATANAKA</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1353,12 +1353,12 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Maia</t>
+          <t>MAIA</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Hawkins</t>
+          <t>HAWKINS</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1368,12 +1368,12 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Shane</t>
+          <t>SHANE</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Herbert</t>
+          <t>HERBERT</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1383,12 +1383,12 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>DANIEL</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Hilfer</t>
+          <t>HILFER</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1398,12 +1398,12 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Todd</t>
+          <t>TODD</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Hill</t>
+          <t>HILL</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1413,12 +1413,12 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Dane</t>
+          <t>DANE</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Holcombe</t>
+          <t>HOLCOMBE</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1428,12 +1428,12 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Colby</t>
+          <t>COLBY</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Hunsaker</t>
+          <t>HUNSAKER</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1443,12 +1443,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Nyla</t>
+          <t>NYLA</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Jacobs</t>
+          <t>JACOBS</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1458,12 +1458,12 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Lesli</t>
+          <t>LESLI</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Jaimes</t>
+          <t>JAIMES</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1473,12 +1473,12 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Matthew</t>
+          <t>MATTHEW</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Jarvis</t>
+          <t>JARVIS</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1488,12 +1488,12 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Marilynn</t>
+          <t>MARILYNN</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Jauregui</t>
+          <t>JAUREGUI</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1503,12 +1503,12 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Frances</t>
+          <t>FRANCES</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Javier</t>
+          <t>JAVIER</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1518,12 +1518,12 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Bailey</t>
+          <t>BAILEY</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>JONES</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1533,12 +1533,12 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Quin'c'allen</t>
+          <t>QUIN'C'ALLEN</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>JONES</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1548,12 +1548,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>RYAN</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>JONES</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1563,12 +1563,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Jamie</t>
+          <t>JAMIE</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Kagy</t>
+          <t>KAGY</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1578,12 +1578,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Gregory</t>
+          <t>GREGORY</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Kettelkamp</t>
+          <t>KETTELKAMP</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1593,12 +1593,12 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Sydney</t>
+          <t>SYDNEY</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Klatt</t>
+          <t>KLATT</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1608,12 +1608,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Sage</t>
+          <t>SAGE</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Klein</t>
+          <t>KLEIN</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1623,12 +1623,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Melanie</t>
+          <t>MELANIE</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Knafla</t>
+          <t>KNAFLA</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1638,12 +1638,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Maxwell</t>
+          <t>MAXWELL</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Krohn</t>
+          <t>KROHN</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1653,12 +1653,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>John Kenneth</t>
+          <t>JOHN KENNETH</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Lauder</t>
+          <t>LAUDER</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1668,12 +1668,12 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>AARON</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Leal</t>
+          <t>LEAL</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1683,12 +1683,12 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Esther</t>
+          <t>ESTHER</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>LEE</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1698,12 +1698,12 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>JAMES</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>LEE</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1713,12 +1713,12 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Jin Sun</t>
+          <t>JIN SUN</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Lee</t>
+          <t>LEE</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1728,12 +1728,12 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Daisy</t>
+          <t>DAISY</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Lengkong</t>
+          <t>LENGKONG</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1743,12 +1743,12 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Sirena</t>
+          <t>SIRENA</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Lepe</t>
+          <t>LEPE</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1758,12 +1758,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Khourtney</t>
+          <t>KHOURTNEY</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Linton</t>
+          <t>LINTON</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1773,12 +1773,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Julia</t>
+          <t>JULIA</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Lomas</t>
+          <t>LOMAS</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1788,12 +1788,12 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Evan</t>
+          <t>EVAN</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Long</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1803,12 +1803,12 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Phoebe</t>
+          <t>PHOEBE</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Long</t>
+          <t>LONG</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1818,12 +1818,12 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Rilee</t>
+          <t>RILEE</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Lopes</t>
+          <t>LOPES</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1833,12 +1833,12 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Araceli</t>
+          <t>ARACELI</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Lozano</t>
+          <t>LOZANO</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1848,12 +1848,12 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Darling</t>
+          <t>DARLING</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Luna</t>
+          <t>LUNA</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1863,12 +1863,12 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Roxanna</t>
+          <t>ROXANNA</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Luna-Barragan</t>
+          <t>LUNA-BARRAGAN</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1878,12 +1878,12 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>ANTHONY</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Marcaida</t>
+          <t>MARCAIDA</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1893,12 +1893,12 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Victor</t>
+          <t>VICTOR</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Marroquin</t>
+          <t>MARROQUIN</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1908,12 +1908,12 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Kira</t>
+          <t>KIRA</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Marshall</t>
+          <t>MARSHALL</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1923,12 +1923,12 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Paula Ann</t>
+          <t>PAULA ANN</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>MARTIN</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1938,12 +1938,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Sebastian</t>
+          <t>SEBASTIAN</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Martin</t>
+          <t>MARTIN</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1953,12 +1953,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Sara</t>
+          <t>SARA</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Mata</t>
+          <t>MATA</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1968,12 +1968,12 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Brent</t>
+          <t>BRENT</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Mayhew</t>
+          <t>MAYHEW</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1983,12 +1983,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Samantha</t>
+          <t>SAMANTHA</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>McKinnon</t>
+          <t>MCKINNON</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1998,12 +1998,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Abigail</t>
+          <t>ABIGAIL</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>McMillen</t>
+          <t>MCMILLEN</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2013,12 +2013,12 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Mccrae</t>
+          <t>MCCRAE</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Medina</t>
+          <t>MEDINA</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2028,12 +2028,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Evelyn</t>
+          <t>EVELYN</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Mejia</t>
+          <t>MEJIA</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2043,27 +2043,27 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Kenichi</t>
+          <t>KENICHI</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Mekaru</t>
+          <t>MEKARU</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>92.69999999999999</v>
+        <v>92.7</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Guadalupe</t>
+          <t>GUADALUPE</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>Menchaca</t>
+          <t>MENCHACA</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2073,12 +2073,12 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Ruth</t>
+          <t>RUTH</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Mercado</t>
+          <t>MERCADO</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2088,12 +2088,12 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Christopher</t>
+          <t>CHRISTOPHER</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Mijares</t>
+          <t>MIJARES</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2103,12 +2103,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>JENNIFER</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Minton</t>
+          <t>MINTON</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2118,12 +2118,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Ian Gabriel</t>
+          <t>IAN GABRIEL</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Mojica</t>
+          <t>MOJICA</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2133,12 +2133,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Alicia</t>
+          <t>ALICIA</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Molina</t>
+          <t>MOLINA</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2148,12 +2148,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Jenna</t>
+          <t>JENNA</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Morigi</t>
+          <t>MORIGI</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2163,12 +2163,12 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Christian</t>
+          <t>CHRISTIAN</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Morrill</t>
+          <t>MORRILL</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2178,12 +2178,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>AARON</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Mostin</t>
+          <t>MOSTIN</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2193,12 +2193,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Andre</t>
+          <t>ANDRE</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Mueller</t>
+          <t>MUELLER</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2208,12 +2208,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Jennifer</t>
+          <t>JENNIFER</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Murillo</t>
+          <t>MURILLO</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2223,12 +2223,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Leshan</t>
+          <t>LESHAN</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Napper</t>
+          <t>NAPPER</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2238,12 +2238,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Ruby</t>
+          <t>RUBY</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Navarro</t>
+          <t>NAVARRO</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2253,12 +2253,12 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Evan</t>
+          <t>EVAN</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Nicol</t>
+          <t>NICOL</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2268,12 +2268,12 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>SARAH</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Omuse</t>
+          <t>OMUSE</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2283,12 +2283,12 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Cristal</t>
+          <t>CRISTAL</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Oropeza</t>
+          <t>OROPEZA</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2298,12 +2298,12 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Miguel</t>
+          <t>MIGUEL</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Ortiz</t>
+          <t>ORTIZ</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2328,12 +2328,12 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Jenifer</t>
+          <t>JENIFER</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>PEREZ</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2343,12 +2343,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Frank</t>
+          <t>FRANK</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>Potter</t>
+          <t>POTTER</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2358,12 +2358,12 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Sarah</t>
+          <t>SARAH</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Powell</t>
+          <t>POWELL</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2373,12 +2373,12 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Guljit</t>
+          <t>GULJIT</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>Rai</t>
+          <t>RAI</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2388,12 +2388,12 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Cole</t>
+          <t>COLE</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Ready</t>
+          <t>READY</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2403,12 +2403,12 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Marlyn</t>
+          <t>MARLYN</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Rectoran</t>
+          <t>RECTORAN</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2418,12 +2418,12 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Raymundo</t>
+          <t>RAYMUNDO</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Reyes</t>
+          <t>REYES</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2433,12 +2433,12 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Vanessa</t>
+          <t>VANESSA</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Rizo</t>
+          <t>RIZO</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2463,12 +2463,12 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Melissa</t>
+          <t>MELISSA</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Rojas</t>
+          <t>ROJAS</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2478,12 +2478,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Syndi</t>
+          <t>SYNDI</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Rosales-Rodriguez</t>
+          <t>ROSALES-RODRIGUEZ</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2493,12 +2493,12 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Brianca</t>
+          <t>BRIANCA</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Ryan</t>
+          <t>RYAN</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2508,12 +2508,12 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Lindsay</t>
+          <t>LINDSAY</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Saker</t>
+          <t>SAKER</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2523,12 +2523,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>MICHAEL</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Saks</t>
+          <t>SAKS</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2538,12 +2538,12 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Alexander</t>
+          <t>ALEXANDER</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Salman</t>
+          <t>SALMAN</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2553,12 +2553,12 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Abigail</t>
+          <t>ABIGAIL</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Sangco</t>
+          <t>SANGCO</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2568,12 +2568,12 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>ANTHONY</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Santich</t>
+          <t>SANTICH</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2583,12 +2583,12 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>JUAN</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Sarmiento</t>
+          <t>SARMIENTO</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2598,12 +2598,12 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Lily</t>
+          <t>LILY</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>shariat</t>
+          <t>SHARIAT</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2613,12 +2613,12 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Penn</t>
+          <t>PENN</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Shelton</t>
+          <t>SHELTON</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2628,12 +2628,12 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>DANIEL</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Shetterly</t>
+          <t>SHETTERLY</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2643,12 +2643,12 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>FRANCIS</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Shih</t>
+          <t>SHIH</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2658,12 +2658,12 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>BRITTANY</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Skinner</t>
+          <t>SKINNER</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2673,12 +2673,12 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Donald</t>
+          <t>DONALD</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Stanciell</t>
+          <t>STANCIELL</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2688,12 +2688,12 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>GEORGE</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Stephan</t>
+          <t>STEPHAN</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2703,12 +2703,12 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>Carly</t>
+          <t>CARLY</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Stidhum</t>
+          <t>STIDHUM</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2718,12 +2718,12 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Adilene</t>
+          <t>ADILENE</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Suarez</t>
+          <t>SUAREZ</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2733,12 +2733,12 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Shemiah</t>
+          <t>SHEMIAH</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Sullivan</t>
+          <t>SULLIVAN</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2748,12 +2748,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Raquel</t>
+          <t>RAQUEL</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Tahvildari</t>
+          <t>TAHVILDARI</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2763,12 +2763,12 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Joseph</t>
+          <t>JOSEPH</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Toews</t>
+          <t>TOEWS</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2778,12 +2778,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>STEPHANIE</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Townsend</t>
+          <t>TOWNSEND</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2793,12 +2793,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Rudy</t>
+          <t>RUDY</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Trejo</t>
+          <t>TREJO</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2808,12 +2808,12 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Alexa</t>
+          <t>ALEXA</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Trogman</t>
+          <t>TROGMAN</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2823,12 +2823,12 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Anthony</t>
+          <t>ANTHONY</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Ugliano</t>
+          <t>UGLIANO</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2838,12 +2838,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Genesis</t>
+          <t>GENESIS</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>Vasquez</t>
+          <t>VASQUEZ</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2853,12 +2853,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Brittany</t>
+          <t>BRITTANY</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Vergara</t>
+          <t>VERGARA</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2868,12 +2868,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Caroline</t>
+          <t>CAROLINE</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Waldman</t>
+          <t>WALDMAN</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2883,12 +2883,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Haiyan</t>
+          <t>HAIYAN</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Wang</t>
+          <t>WANG</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2898,12 +2898,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Allana</t>
+          <t>ALLANA</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Wenger Vidovich</t>
+          <t>WENGER VIDOVICH</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2913,12 +2913,12 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Samantha</t>
+          <t>SAMANTHA</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Whitford</t>
+          <t>WHITFORD</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2928,12 +2928,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Kevin</t>
+          <t>KEVIN</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Zheng</t>
+          <t>ZHENG</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2943,12 +2943,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Francis</t>
+          <t>FRANCIS</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Zumbro</t>
+          <t>ZUMBRO</t>
         </is>
       </c>
       <c r="C168" t="n">

</xml_diff>